<commit_message>
fix: remove unecessary file
</commit_message>
<xml_diff>
--- a/wetezos/evidence.xlsx
+++ b/wetezos/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28840" windowHeight="14900" firstSheet="14" activeTab="25"/>
+    <workbookView windowWidth="28840" windowHeight="14900" firstSheet="14" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="94">
   <si>
     <t>TeamName</t>
   </si>
@@ -209,10 +209,28 @@
     <t>1B866E686BF01A9F6001C888097E16BADF87E393786F65C6FA80327373F78206</t>
   </si>
   <si>
-    <t>9A4B48425D1739A860E4C38B65E5A14E590B826F55D41C2BFE17B5851AEDBC4F</t>
-  </si>
-  <si>
-    <t>94B45E8F19778416D277224F3914987021459F30DEAF461430E82ECE0350E5F4</t>
+    <t>4C89CAE7A9E580E102138FD2FB306C9BD3FD6F0E70CCE67FDAE9521876910C29</t>
+  </si>
+  <si>
+    <t>CFAC93E401B4673244A8592EBEBA217E2725512754ACEFFD2985ECDA8C7D924A</t>
+  </si>
+  <si>
+    <t>2CD26A30766C37E9C2C0F883F7F218861F135087EFCC8CDC70F8F8A0ADD1C4F1</t>
+  </si>
+  <si>
+    <t>27515F048768A6BE4EEF394EE87EE25E8335633CDFA1312B513D2862D669E69A</t>
+  </si>
+  <si>
+    <t>66BDA2C704E0B80987594AE011DD86C6ECDFB3007FA9818BE5C64BC8D3C83E84</t>
+  </si>
+  <si>
+    <t>933BF6906CDAB12BC5ECFB0075CC04A598A80B3992AF7F985C22D49FB59B76B3</t>
+  </si>
+  <si>
+    <t>2D0D18A39DB9C0253AE4B1548A7DCCA6C0D180B4D855408EFC3BAAF0B0A1360C</t>
+  </si>
+  <si>
+    <t>557DCC98EAA45AEB69D0331AB5FADDE5FAEAB3A56290544CD6ED636962DFF9A5</t>
   </si>
   <si>
     <t>82199F282E69BB718F669B5F74CEB7020BEAD7AE05C40034C16270FFF2E00156</t>
@@ -275,10 +293,10 @@
     <t>3A0E0506CF1D4411F25CB925C03989131C3C8130BC241737B03CFF1C25823699</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
+    <t>AAB879A15B90EF2A6F0DA041E42B725505DD144048E2EFCFA690C9D32B4A067F</t>
+  </si>
+  <si>
+    <t>E30E2E9B3292E361F4D226D6CEDC438B9131951E5DA64CF89FCEAA8EB511E0E7</t>
   </si>
   <si>
     <t>40712DBA2C08AC67030D1429FC471FD6D493F97EA4556C8F77B1A6415C80122D</t>
@@ -312,8 +330,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -343,6 +361,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -356,18 +381,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -387,33 +427,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,16 +442,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,22 +460,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -472,6 +473,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -479,12 +488,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -519,25 +537,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,13 +615,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,127 +699,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,18 +747,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -760,21 +767,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -786,6 +778,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -807,157 +808,174 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1688,8 +1706,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1715,18 +1733,25 @@
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1745,7 +1770,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1764,26 +1789,32 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1821,7 +1852,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
@@ -1829,7 +1860,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>48</v>
@@ -1837,7 +1868,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -1845,7 +1876,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>48</v>
@@ -1888,7 +1919,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
@@ -1896,7 +1927,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>30</v>
@@ -1904,7 +1935,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>50</v>
@@ -1912,7 +1943,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -1990,7 +2021,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
@@ -1998,7 +2029,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>48</v>
@@ -2006,7 +2037,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>27</v>
@@ -2014,7 +2045,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>50</v>
@@ -2022,7 +2053,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
@@ -2030,7 +2061,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>48</v>
@@ -2094,7 +2125,7 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
@@ -2102,7 +2133,7 @@
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>50</v>
@@ -2110,7 +2141,7 @@
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>48</v>
@@ -2118,7 +2149,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -2126,7 +2157,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>48</v>
@@ -2134,7 +2165,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>50</v>
@@ -2154,12 +2185,12 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="45.4615384615385" style="3" customWidth="1"/>
+    <col min="1" max="1" width="95.8461538461538" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="1:1">
@@ -2169,12 +2200,12 @@
     </row>
     <row r="2" ht="16.4" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2206,12 +2237,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2243,12 +2274,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2280,12 +2311,12 @@
     </row>
     <row r="2" ht="17.25" customHeight="1" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2299,8 +2330,8 @@
   <sheetPr/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2"/>
@@ -2315,12 +2346,12 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>